<commit_message>
Spalten A-E des Tabellenkalkulationsprogramms werden gesetzt
  - Make wird vorne ein ''|'' einbauen (wie bereits zuvor das letzte)
  - Spalten A-E werden gesetzt
</commit_message>
<xml_diff>
--- a/input/00-beispiel.xlsx
+++ b/input/00-beispiel.xlsx
@@ -131,7 +131,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -258,53 +258,52 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1048576"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="42.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="37.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="33.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="37.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="33.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16383" min="7" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="205.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>